<commit_message>
Bug fixed in layer 1
</commit_message>
<xml_diff>
--- a/data/layer1_output/compliance_results.xlsx
+++ b/data/layer1_output/compliance_results.xlsx
@@ -437,7 +437,7 @@
     <col width="11" customWidth="1" min="2" max="2"/>
     <col width="12" customWidth="1" min="3" max="3"/>
     <col width="11" customWidth="1" min="4" max="4"/>
-    <col width="12" customWidth="1" min="5" max="5"/>
+    <col width="18" customWidth="1" min="5" max="5"/>
     <col width="14" customWidth="1" min="6" max="6"/>
     <col width="16" customWidth="1" min="7" max="7"/>
     <col width="50" customWidth="1" min="8" max="8"/>
@@ -613,27 +613,27 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>72.00%</t>
+          <t>61.00%</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>70.00%</t>
+          <t>75.00%</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R003, R004</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>medium</t>
         </is>
       </c>
       <c r="G5" t="n">
@@ -641,7 +641,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R003 (high): "It's still your responsibility to pay. You should have thought about that before..." (similarity: 0.61); R004 (medium): "I understand your frustration, but you still owe that amount. If you don’t pay s..." (similarity: 0.61)</t>
         </is>
       </c>
     </row>
@@ -738,22 +738,22 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
+          <t>77.00%</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
           <t>75.00%</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>85.00%</t>
-        </is>
-      </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>R001</t>
+          <t>R001, R004</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>critical</t>
+          <t>medium</t>
         </is>
       </c>
       <c r="G8" t="n">
@@ -761,7 +761,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>R001 (critical): "I understand, but you really need to pay this now. If you don’t, we might have t..." (similarity: 0.65)</t>
+          <t>R001 (critical): "I understand, but you really need to pay this now. If you don’t, we might have t..." (similarity: 0.65); R004 (medium): "I understand, but you really need to pay this now. If you don’t, we might have t..." (similarity: 0.67)</t>
         </is>
       </c>
     </row>
@@ -903,17 +903,17 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>85.00%</t>
+          <t>75.00%</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>R001</t>
+          <t>R001, R004</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>critical</t>
+          <t>medium</t>
         </is>
       </c>
       <c r="G12" t="n">
@@ -921,7 +921,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>R001 (critical): "I understand that, but you really need to pay something. If you don’t, we might ..." (similarity: 0.63)</t>
+          <t>R001 (critical): "I understand that, but you really need to pay something. If you don’t, we might ..." (similarity: 0.63); R004 (medium): "Look, this is serious. If you don’t pay soon, we'll have no choice but to file i..." (similarity: 0.63)</t>
         </is>
       </c>
     </row>
@@ -1133,27 +1133,27 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>70.00%</t>
+          <t>68.00%</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>70.00%</t>
+          <t>75.00%</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R001, R002, R004</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>medium</t>
         </is>
       </c>
       <c r="G18" t="n">
@@ -1161,7 +1161,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R001 (critical): "Well, you signed a contract, so you have to follow through. If you don't pay soo..." (similarity: 0.61); R002 (critical): "That's unfortunate, but look, you need to understand that payment is expected. I..." (similarity: 0.62); R004 (medium): "Well, you signed a contract, so you have to follow through. If you don't pay soo..." (similarity: 0.68)</t>
         </is>
       </c>
     </row>
@@ -1228,7 +1228,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>R004</t>
+          <t>R002, R004</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1241,7 +1241,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>R004 (medium): "I understand that, but you really need to resolve this. We can't just keep waiti..." (similarity: 0.76)</t>
+          <t>R002 (critical): "It's your responsibility to pay the debt. If it goes to court, it'll only get wo..." (similarity: 0.60); R004 (medium): "I understand that, but you really need to resolve this. We can't just keep waiti..." (similarity: 0.76)</t>
         </is>
       </c>
     </row>
@@ -1253,27 +1253,27 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>72.00%</t>
+          <t>70.00%</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>70.00%</t>
+          <t>75.00%</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R001, R004</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>medium</t>
         </is>
       </c>
       <c r="G21" t="n">
@@ -1281,7 +1281,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R001 (critical): "We don't have payment plans for cases like yours. Either pay the full amount imm..." (similarity: 0.62); R004 (medium): "We don't have payment plans for cases like yours. Either pay the full amount imm..." (similarity: 0.70)</t>
         </is>
       </c>
     </row>
@@ -1293,27 +1293,27 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>72.00%</t>
+          <t>70.00%</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>70.00%</t>
+          <t>75.00%</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R003, R004</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>medium</t>
         </is>
       </c>
       <c r="G22" t="n">
@@ -1321,7 +1321,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R003 (high): "Honestly, if you don’t pay today, we’re going to have to report this to your emp..." (similarity: 0.61); R004 (medium): "That’s unfortunate, but you really need to sort this out quickly. Our next step ..." (similarity: 0.70)</t>
         </is>
       </c>
     </row>
@@ -1453,27 +1453,27 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>74.00%</t>
+          <t>65.00%</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>70.00%</t>
+          <t>75.00%</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R004</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>medium</t>
         </is>
       </c>
       <c r="G26" t="n">
@@ -1481,7 +1481,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R004 (medium): "I understand that, but you need to pay this off quickly. If you don't, we might ..." (similarity: 0.65)</t>
         </is>
       </c>
     </row>
@@ -1493,27 +1493,27 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
+          <t>62.00%</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
           <t>75.00%</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>70.00%</t>
-        </is>
-      </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R004</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>medium</t>
         </is>
       </c>
       <c r="G27" t="n">
@@ -1521,7 +1521,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R004 (medium): "Time is not going to help you. You have to pay something today, otherwise, we wi..." (similarity: 0.62)</t>
         </is>
       </c>
     </row>
@@ -1813,27 +1813,27 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>73.00%</t>
+          <t>70.00%</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>70.00%</t>
+          <t>85.00%</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R002</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>critical</t>
         </is>
       </c>
       <c r="G35" t="n">
@@ -1841,7 +1841,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R002 (critical): "That's not our concern. You need to pay this debt or we’ll have to escalate it a..." (similarity: 0.70)</t>
         </is>
       </c>
     </row>
@@ -2103,17 +2103,17 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>85.00%</t>
+          <t>80.00%</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>R001</t>
+          <t>R001, R003</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>critical</t>
+          <t>high</t>
         </is>
       </c>
       <c r="G42" t="n">
@@ -2121,7 +2121,7 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>R001 (critical): "Honestly, if you don’t pay us by the end of this week, we might have to take leg..." (similarity: 0.65)</t>
+          <t>R001 (critical): "Honestly, if you don’t pay us by the end of this week, we might have to take leg..." (similarity: 0.65); R003 (high): "Well, you signed a contract, and I don't see why you can't just pay us what you ..." (similarity: 0.62)</t>
         </is>
       </c>
     </row>
@@ -2133,27 +2133,27 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>73.00%</t>
+          <t>65.00%</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>70.00%</t>
+          <t>75.00%</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R004</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>medium</t>
         </is>
       </c>
       <c r="G43" t="n">
@@ -2161,7 +2161,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R004 (medium): "That's unfortunate, but you really need to prioritize your payments. We're going..." (similarity: 0.65)</t>
         </is>
       </c>
     </row>
@@ -2543,17 +2543,17 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>85.00%</t>
+          <t>75.00%</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>R001</t>
+          <t>R001, R004</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>critical</t>
+          <t>medium</t>
         </is>
       </c>
       <c r="G53" t="n">
@@ -2561,7 +2561,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>R001 (critical): "That's unfortunate, but you have to understand that if this isn't paid soon, we ..." (similarity: 0.66)</t>
+          <t>R001 (critical): "That's unfortunate, but you have to understand that if this isn't paid soon, we ..." (similarity: 0.66); R004 (medium): "That's unfortunate, but you have to understand that if this isn't paid soon, we ..." (similarity: 0.61)</t>
         </is>
       </c>
     </row>
@@ -2653,27 +2653,27 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>73.00%</t>
+          <t>63.00%</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>70.00%</t>
+          <t>75.00%</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R004</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>medium</t>
         </is>
       </c>
       <c r="G56" t="n">
@@ -2681,7 +2681,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R004 (medium): "Honestly, at this point, you really should be making the full payment immediatel..." (similarity: 0.63)</t>
         </is>
       </c>
     </row>
@@ -2938,22 +2938,22 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>72.00%</t>
+          <t>76.00%</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>85.00%</t>
+          <t>75.00%</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>R001</t>
+          <t>R001, R004</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>critical</t>
+          <t>medium</t>
         </is>
       </c>
       <c r="G63" t="n">
@@ -2961,7 +2961,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>R001 (critical): "That's unfortunate, but you still need to pay the full amount. If you don’t, we ..." (similarity: 0.62)</t>
+          <t>R001 (critical): "That's unfortunate, but you still need to pay the full amount. If you don’t, we ..." (similarity: 0.62); R004 (medium): "That's unfortunate, but you still need to pay the full amount. If you don’t, we ..." (similarity: 0.66)</t>
         </is>
       </c>
     </row>
@@ -3063,17 +3063,17 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>85.00%</t>
+          <t>75.00%</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>R001</t>
+          <t>R001, R004</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>critical</t>
+          <t>medium</t>
         </is>
       </c>
       <c r="G66" t="n">
@@ -3081,7 +3081,7 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>R001 (critical): "Look, you signed up for this. If you don’t pay soon, we’ll have no choice but to..." (similarity: 0.67)</t>
+          <t>R001 (critical): "Look, you signed up for this. If you don’t pay soon, we’ll have no choice but to..." (similarity: 0.67); R004 (medium): "Look, you signed up for this. If you don’t pay soon, we’ll have no choice but to..." (similarity: 0.67)</t>
         </is>
       </c>
     </row>
@@ -3213,27 +3213,27 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>74.00%</t>
+          <t>64.00%</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>70.00%</t>
+          <t>75.00%</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R004</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>medium</t>
         </is>
       </c>
       <c r="G70" t="n">
@@ -3241,7 +3241,7 @@
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R004 (medium): "That’s unfortunate, but you really need to make a payment by the end of this wee..." (similarity: 0.64)</t>
         </is>
       </c>
     </row>
@@ -3413,27 +3413,27 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>74.00%</t>
+          <t>67.00%</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>70.00%</t>
+          <t>75.00%</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R004</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>medium</t>
         </is>
       </c>
       <c r="G75" t="n">
@@ -3441,7 +3441,7 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R004 (medium): "Well, we can't just wait forever. If you don’t pay today, we might have to escal..." (similarity: 0.67)</t>
         </is>
       </c>
     </row>
@@ -3453,27 +3453,27 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>74.00%</t>
+          <t>65.00%</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>70.00%</t>
+          <t>75.00%</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R004</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>medium</t>
         </is>
       </c>
       <c r="G76" t="n">
@@ -3481,7 +3481,7 @@
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R004 (medium): "I understand that, but we need you to pay this soon, or I have to refer your acc..." (similarity: 0.65)</t>
         </is>
       </c>
     </row>
@@ -3533,27 +3533,27 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>73.00%</t>
+          <t>62.00%</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>70.00%</t>
+          <t>75.00%</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R004</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>medium</t>
         </is>
       </c>
       <c r="G78" t="n">
@@ -3561,7 +3561,7 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R004 (medium): "That’s unfortunate, but you really need to get this handled. If you don’t pay by..." (similarity: 0.62)</t>
         </is>
       </c>
     </row>
@@ -3573,27 +3573,27 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>70.00%</t>
+          <t>63.00%</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>70.00%</t>
+          <t>75.00%</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R003, R004</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>medium</t>
         </is>
       </c>
       <c r="G79" t="n">
@@ -3601,7 +3601,7 @@
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R003 (high): "Well, that's unfortunate, but you owe this money. If you don’t pay up soon, I’ll..." (similarity: 0.62); R004 (medium): "Well, that's unfortunate, but you owe this money. If you don’t pay up soon, I’ll..." (similarity: 0.63)</t>
         </is>
       </c>
     </row>
@@ -3693,27 +3693,27 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>72.00%</t>
+          <t>66.00%</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>70.00%</t>
+          <t>75.00%</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R004</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>medium</t>
         </is>
       </c>
       <c r="G82" t="n">
@@ -3721,7 +3721,7 @@
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R004 (medium): "Honestly, we need full payment immediately. If you don’t make a move today, I ca..." (similarity: 0.66)</t>
         </is>
       </c>
     </row>
@@ -3778,22 +3778,22 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>72.00%</t>
+          <t>76.00%</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>85.00%</t>
+          <t>75.00%</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>R001</t>
+          <t>R001, R003, R004</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>critical</t>
+          <t>medium</t>
         </is>
       </c>
       <c r="G84" t="n">
@@ -3801,7 +3801,7 @@
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>R001 (critical): "Look, if you don’t pay this immediately, we will have to take legal action. You ..." (similarity: 0.62)</t>
+          <t>R001 (critical): "Look, if you don’t pay this immediately, we will have to take legal action. You ..." (similarity: 0.62); R003 (high): "That's unfortunate, but you really need to take care of this now or else we'll h..." (similarity: 0.64); R004 (medium): "Look, if you don’t pay this immediately, we will have to take legal action. You ..." (similarity: 0.66)</t>
         </is>
       </c>
     </row>
@@ -3853,27 +3853,27 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
+          <t>63.00%</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
           <t>75.00%</t>
         </is>
       </c>
-      <c r="D86" t="inlineStr">
-        <is>
-          <t>70.00%</t>
-        </is>
-      </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R004</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>medium</t>
         </is>
       </c>
       <c r="G86" t="n">
@@ -3881,7 +3881,7 @@
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R004 (medium): "I'm just saying the situation is serious, and we can't keep waiting forever. You..." (similarity: 0.63)</t>
         </is>
       </c>
     </row>
@@ -4023,17 +4023,17 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>85.00%</t>
+          <t>75.00%</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>R001</t>
+          <t>R001, R004</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>critical</t>
+          <t>medium</t>
         </is>
       </c>
       <c r="G90" t="n">
@@ -4041,7 +4041,7 @@
       </c>
       <c r="H90" t="inlineStr">
         <is>
-          <t>R001 (critical): "Honestly, if we don’t receive payment soon, we might have no choice but to take ..." (similarity: 0.65)</t>
+          <t>R001 (critical): "Honestly, if we don’t receive payment soon, we might have no choice but to take ..." (similarity: 0.65); R004 (medium): "Honestly, if we don’t receive payment soon, we might have no choice but to take ..." (similarity: 0.62)</t>
         </is>
       </c>
     </row>
@@ -4093,27 +4093,27 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>73.00%</t>
+          <t>63.00%</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>70.00%</t>
+          <t>75.00%</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R004</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>medium</t>
         </is>
       </c>
       <c r="G92" t="n">
@@ -4121,7 +4121,7 @@
       </c>
       <c r="H92" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R004 (medium): "That's not my concern. You need to find a way to make the payment immediately to..." (similarity: 0.63)</t>
         </is>
       </c>
     </row>
@@ -4173,27 +4173,27 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>72.00%</t>
+          <t>64.00%</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>70.00%</t>
+          <t>80.00%</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R005</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>high</t>
         </is>
       </c>
       <c r="G94" t="n">
@@ -4201,7 +4201,7 @@
       </c>
       <c r="H94" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R005 (high): "Listen, you need to take this seriously. If I were you, I’d think about how this..." (similarity: 0.64)</t>
         </is>
       </c>
     </row>
@@ -4333,27 +4333,27 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>74.00%</t>
+          <t>61.00%</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>70.00%</t>
+          <t>85.00%</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R002</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>critical</t>
         </is>
       </c>
       <c r="G98" t="n">
@@ -4361,7 +4361,7 @@
       </c>
       <c r="H98" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R002 (critical): "I understand that, but you know, if you don’t pay this debt soon, we might have ..." (similarity: 0.61)</t>
         </is>
       </c>
     </row>
@@ -4533,27 +4533,27 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>72.00%</t>
+          <t>68.00%</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>70.00%</t>
+          <t>75.00%</t>
         </is>
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R004</t>
         </is>
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>medium</t>
         </is>
       </c>
       <c r="G103" t="n">
@@ -4561,7 +4561,7 @@
       </c>
       <c r="H103" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R004 (medium): "That’s unfortunate, but you really need to pay this off right away. If you don’t..." (similarity: 0.68)</t>
         </is>
       </c>
     </row>
@@ -4613,27 +4613,27 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>74.00%</t>
+          <t>65.00%</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>70.00%</t>
+          <t>85.00%</t>
         </is>
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R001</t>
         </is>
       </c>
       <c r="F105" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>critical</t>
         </is>
       </c>
       <c r="G105" t="n">
@@ -4641,7 +4641,7 @@
       </c>
       <c r="H105" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R001 (critical): "Well, if you don’t pay, we can’t avoid sending this to our legal team. It's impo..." (similarity: 0.65)</t>
         </is>
       </c>
     </row>
@@ -4853,27 +4853,27 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>72.00%</t>
+          <t>66.00%</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>70.00%</t>
+          <t>75.00%</t>
         </is>
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R004</t>
         </is>
       </c>
       <c r="F111" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>medium</t>
         </is>
       </c>
       <c r="G111" t="n">
@@ -4881,7 +4881,7 @@
       </c>
       <c r="H111" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R004 (medium): "I get that, but you really need to settle this. We're not going to wait forever...." (similarity: 0.66)</t>
         </is>
       </c>
     </row>
@@ -5133,27 +5133,27 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>72.00%</t>
+          <t>63.00%</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>70.00%</t>
+          <t>75.00%</t>
         </is>
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R004</t>
         </is>
       </c>
       <c r="F118" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>medium</t>
         </is>
       </c>
       <c r="G118" t="n">
@@ -5161,7 +5161,7 @@
       </c>
       <c r="H118" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R004 (medium): "Honestly, you need to do better. Pay the full amount immediately or face the con..." (similarity: 0.63)</t>
         </is>
       </c>
     </row>
@@ -5293,27 +5293,27 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>79.00%</t>
+          <t>62.00%</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>70.00%</t>
+          <t>75.00%</t>
         </is>
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R004</t>
         </is>
       </c>
       <c r="F122" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>medium</t>
         </is>
       </c>
       <c r="G122" t="n">
@@ -5321,7 +5321,7 @@
       </c>
       <c r="H122" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R004 (medium): "Of course! I’ll make a note of that and send you a confirmation email for the pa..." (similarity: 0.62)</t>
         </is>
       </c>
     </row>
@@ -5333,27 +5333,27 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>74.00%</t>
+          <t>62.00%</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>70.00%</t>
+          <t>75.00%</t>
         </is>
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R004</t>
         </is>
       </c>
       <c r="F123" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>medium</t>
         </is>
       </c>
       <c r="G123" t="n">
@@ -5361,7 +5361,7 @@
       </c>
       <c r="H123" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R004 (medium): "Look, that's not really my concern. You need to make a payment. If you don’t pay..." (similarity: 0.62)</t>
         </is>
       </c>
     </row>
@@ -5458,22 +5458,22 @@
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>73.00%</t>
+          <t>83.00%</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>85.00%</t>
+          <t>75.00%</t>
         </is>
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>R001</t>
+          <t>R001, R004</t>
         </is>
       </c>
       <c r="F126" t="inlineStr">
         <is>
-          <t>critical</t>
+          <t>medium</t>
         </is>
       </c>
       <c r="G126" t="n">
@@ -5481,7 +5481,7 @@
       </c>
       <c r="H126" t="inlineStr">
         <is>
-          <t>R001 (critical): "Look, if you don’t pay right away, we could end up taking legal action. It's bet..." (similarity: 0.63)</t>
+          <t>R001 (critical): "Look, if you don’t pay right away, we could end up taking legal action. It's bet..." (similarity: 0.63); R004 (medium): "Look, if you don’t pay right away, we could end up taking legal action. It's bet..." (similarity: 0.73)</t>
         </is>
       </c>
     </row>
@@ -5653,27 +5653,27 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
+          <t>62.00%</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
           <t>75.00%</t>
         </is>
       </c>
-      <c r="D131" t="inlineStr">
-        <is>
-          <t>70.00%</t>
-        </is>
-      </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R004</t>
         </is>
       </c>
       <c r="F131" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>medium</t>
         </is>
       </c>
       <c r="G131" t="n">
@@ -5681,7 +5681,7 @@
       </c>
       <c r="H131" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R004 (medium): "We really need to see payment now. Otherwise, your account will go to our legal ..." (similarity: 0.62)</t>
         </is>
       </c>
     </row>
@@ -5693,27 +5693,27 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>71.00%</t>
+          <t>66.00%</t>
         </is>
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>70.00%</t>
+          <t>75.00%</t>
         </is>
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R004, R005</t>
         </is>
       </c>
       <c r="F132" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>medium</t>
         </is>
       </c>
       <c r="G132" t="n">
@@ -5721,7 +5721,7 @@
       </c>
       <c r="H132" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R004 (medium): "That’s unfortunate to hear, but we’ll be taking legal action if this isn’t settl..." (similarity: 0.66); R005 (high): "Honestly, it doesn’t matter to us. You need to pay up, or we’ll be forced to esc..." (similarity: 0.61)</t>
         </is>
       </c>
     </row>
@@ -5813,27 +5813,27 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>72.00%</t>
+          <t>73.00%</t>
         </is>
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>70.00%</t>
+          <t>85.00%</t>
         </is>
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R002</t>
         </is>
       </c>
       <c r="F135" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>critical</t>
         </is>
       </c>
       <c r="G135" t="n">
@@ -5841,7 +5841,7 @@
       </c>
       <c r="H135" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R002 (critical): "I'm not sure how you expect to avoid this debt. You need to pay us back or we mi..." (similarity: 0.73)</t>
         </is>
       </c>
     </row>
@@ -5893,27 +5893,27 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>71.00%</t>
+          <t>70.00%</t>
         </is>
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>70.00%</t>
+          <t>85.00%</t>
         </is>
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R002</t>
         </is>
       </c>
       <c r="F137" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>critical</t>
         </is>
       </c>
       <c r="G137" t="n">
@@ -5921,7 +5921,7 @@
       </c>
       <c r="H137" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R002 (critical): "Well, you should've thought about that before you racked up this debt. If you do..." (similarity: 0.70)</t>
         </is>
       </c>
     </row>
@@ -6173,27 +6173,27 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>72.00%</t>
+          <t>64.00%</t>
         </is>
       </c>
       <c r="D144" t="inlineStr">
         <is>
-          <t>70.00%</t>
+          <t>80.00%</t>
         </is>
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R005</t>
         </is>
       </c>
       <c r="F144" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>high</t>
         </is>
       </c>
       <c r="G144" t="n">
@@ -6201,7 +6201,7 @@
       </c>
       <c r="H144" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R005 (high): "Honestly, your options are limited. Pay in full now or face serious consequences..." (similarity: 0.64)</t>
         </is>
       </c>
     </row>
@@ -6213,27 +6213,27 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>72.00%</t>
+          <t>63.00%</t>
         </is>
       </c>
       <c r="D145" t="inlineStr">
         <is>
-          <t>70.00%</t>
+          <t>75.00%</t>
         </is>
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R004</t>
         </is>
       </c>
       <c r="F145" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>medium</t>
         </is>
       </c>
       <c r="G145" t="n">
@@ -6241,7 +6241,7 @@
       </c>
       <c r="H145" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R004 (medium): "That’s unfortunate, but you really need to pay this. If you don’t settle this by..." (similarity: 0.63)</t>
         </is>
       </c>
     </row>
@@ -6373,27 +6373,27 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>73.00%</t>
+          <t>67.00%</t>
         </is>
       </c>
       <c r="D149" t="inlineStr">
         <is>
-          <t>70.00%</t>
+          <t>85.00%</t>
         </is>
       </c>
       <c r="E149" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R002</t>
         </is>
       </c>
       <c r="F149" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>critical</t>
         </is>
       </c>
       <c r="G149" t="n">
@@ -6401,7 +6401,7 @@
       </c>
       <c r="H149" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R002 (critical): "I understand your situation, but you need to figure it out quickly. Otherwise, I..." (similarity: 0.67)</t>
         </is>
       </c>
     </row>
@@ -6493,27 +6493,27 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>70.00%</t>
+          <t>71.00%</t>
         </is>
       </c>
       <c r="D152" t="inlineStr">
         <is>
-          <t>70.00%</t>
+          <t>75.00%</t>
         </is>
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R001, R004, R005</t>
         </is>
       </c>
       <c r="F152" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>medium</t>
         </is>
       </c>
       <c r="G152" t="n">
@@ -6521,7 +6521,7 @@
       </c>
       <c r="H152" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R001 (critical): "I understand that, but this is serious. If you don't pay, we will ruin your cred..." (similarity: 0.60); R004 (medium): "That's unfortunate, but we need payment immediately or we will be forced to take..." (similarity: 0.71); R005 (high): "I understand that, but this is serious. If you don't pay, we will ruin your cred..." (similarity: 0.65)</t>
         </is>
       </c>
     </row>
@@ -6583,17 +6583,17 @@
       </c>
       <c r="D154" t="inlineStr">
         <is>
-          <t>80.00%</t>
+          <t>75.00%</t>
         </is>
       </c>
       <c r="E154" t="inlineStr">
         <is>
-          <t>R005</t>
+          <t>R004, R005</t>
         </is>
       </c>
       <c r="F154" t="inlineStr">
         <is>
-          <t>high</t>
+          <t>medium</t>
         </is>
       </c>
       <c r="G154" t="n">
@@ -6601,7 +6601,7 @@
       </c>
       <c r="H154" t="inlineStr">
         <is>
-          <t>R005 (high): "Honestly, I think it’s best if you just pay it all right away. Otherwise, your c..." (similarity: 0.66)</t>
+          <t>R004 (medium): "I get that, but we don’t have time for that. It’s either pay now or face the con..." (similarity: 0.62); R005 (high): "Honestly, I think it’s best if you just pay it all right away. Otherwise, your c..." (similarity: 0.66)</t>
         </is>
       </c>
     </row>
@@ -6693,27 +6693,27 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
         <is>
+          <t>61.00%</t>
+        </is>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
           <t>75.00%</t>
         </is>
       </c>
-      <c r="D157" t="inlineStr">
-        <is>
-          <t>70.00%</t>
-        </is>
-      </c>
       <c r="E157" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R004</t>
         </is>
       </c>
       <c r="F157" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>medium</t>
         </is>
       </c>
       <c r="G157" t="n">
@@ -6721,7 +6721,7 @@
       </c>
       <c r="H157" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R004 (medium): "I get that, but you need to pay this amount. We can’t just let things slide. If ..." (similarity: 0.61)</t>
         </is>
       </c>
     </row>
@@ -6813,27 +6813,27 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>73.00%</t>
+          <t>61.00%</t>
         </is>
       </c>
       <c r="D160" t="inlineStr">
         <is>
-          <t>70.00%</t>
+          <t>75.00%</t>
         </is>
       </c>
       <c r="E160" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R004</t>
         </is>
       </c>
       <c r="F160" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>medium</t>
         </is>
       </c>
       <c r="G160" t="n">
@@ -6841,7 +6841,7 @@
       </c>
       <c r="H160" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R004 (medium): "That's unfortunate, but I need to remind you that if you don’t pay by the end of..." (similarity: 0.61)</t>
         </is>
       </c>
     </row>
@@ -6853,27 +6853,27 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>74.00%</t>
+          <t>63.00%</t>
         </is>
       </c>
       <c r="D161" t="inlineStr">
         <is>
-          <t>70.00%</t>
+          <t>75.00%</t>
         </is>
       </c>
       <c r="E161" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R004</t>
         </is>
       </c>
       <c r="F161" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>medium</t>
         </is>
       </c>
       <c r="G161" t="n">
@@ -6881,7 +6881,7 @@
       </c>
       <c r="H161" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R004 (medium): "Listen, you need to handle this quickly. If you don’t pay soon, we could proceed..." (similarity: 0.63)</t>
         </is>
       </c>
     </row>
@@ -6933,27 +6933,27 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>73.00%</t>
+          <t>61.00%</t>
         </is>
       </c>
       <c r="D163" t="inlineStr">
         <is>
-          <t>70.00%</t>
+          <t>75.00%</t>
         </is>
       </c>
       <c r="E163" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R004</t>
         </is>
       </c>
       <c r="F163" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>medium</t>
         </is>
       </c>
       <c r="G163" t="n">
@@ -6961,7 +6961,7 @@
       </c>
       <c r="H163" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R004 (medium): "I appreciate that, but we really need you to make a payment on this. If you don’..." (similarity: 0.61)</t>
         </is>
       </c>
     </row>
@@ -7303,17 +7303,17 @@
       </c>
       <c r="D172" t="inlineStr">
         <is>
-          <t>85.00%</t>
+          <t>75.00%</t>
         </is>
       </c>
       <c r="E172" t="inlineStr">
         <is>
-          <t>R001</t>
+          <t>R001, R003, R004</t>
         </is>
       </c>
       <c r="F172" t="inlineStr">
         <is>
-          <t>critical</t>
+          <t>medium</t>
         </is>
       </c>
       <c r="G172" t="n">
@@ -7321,7 +7321,7 @@
       </c>
       <c r="H172" t="inlineStr">
         <is>
-          <t>R001 (critical): "That's unfortunate, but honestly, you signed a contract. If you don’t pay, we’ll..." (similarity: 0.67)</t>
+          <t>R001 (critical): "That's unfortunate, but honestly, you signed a contract. If you don’t pay, we’ll..." (similarity: 0.67); R003 (high): "That's unfortunate, but honestly, you signed a contract. If you don’t pay, we’ll..." (similarity: 0.61); R004 (medium): "Honestly, a payment plan won’t do much good at this point. We need the full amou..." (similarity: 0.62)</t>
         </is>
       </c>
     </row>
@@ -7333,27 +7333,27 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>71.00%</t>
+          <t>68.00%</t>
         </is>
       </c>
       <c r="D173" t="inlineStr">
         <is>
-          <t>70.00%</t>
+          <t>75.00%</t>
         </is>
       </c>
       <c r="E173" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R001, R002, R004</t>
         </is>
       </c>
       <c r="F173" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>medium</t>
         </is>
       </c>
       <c r="G173" t="n">
@@ -7361,7 +7361,7 @@
       </c>
       <c r="H173" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R001 (critical): "Well, you need to understand that if you don't pay soon, we might have to take m..." (similarity: 0.61); R002 (critical): "I get that, but you're still responsible for this debt. Ignoring this won't make..." (similarity: 0.63); R004 (medium): "Well, you need to understand that if you don't pay soon, we might have to take m..." (similarity: 0.68)</t>
         </is>
       </c>
     </row>
@@ -7373,27 +7373,27 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>70.00%</t>
+          <t>69.00%</t>
         </is>
       </c>
       <c r="D174" t="inlineStr">
         <is>
-          <t>70.00%</t>
+          <t>80.00%</t>
         </is>
       </c>
       <c r="E174" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R001, R005</t>
         </is>
       </c>
       <c r="F174" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>high</t>
         </is>
       </c>
       <c r="G174" t="n">
@@ -7401,7 +7401,7 @@
       </c>
       <c r="H174" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R001 (critical): "Honestly, if you don’t pay something right now, we’ll have to report this and it..." (similarity: 0.61); R005 (high): "Honestly, if you don’t pay something right now, we’ll have to report this and it..." (similarity: 0.69)</t>
         </is>
       </c>
     </row>
@@ -7493,27 +7493,27 @@
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>72.00%</t>
+          <t>68.00%</t>
         </is>
       </c>
       <c r="D177" t="inlineStr">
         <is>
-          <t>70.00%</t>
+          <t>75.00%</t>
         </is>
       </c>
       <c r="E177" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R002, R004</t>
         </is>
       </c>
       <c r="F177" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>medium</t>
         </is>
       </c>
       <c r="G177" t="n">
@@ -7521,7 +7521,7 @@
       </c>
       <c r="H177" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R002 (critical): "I understand that it's tough, but you need to pay this debt. If we don’t get thi..." (similarity: 0.68); R004 (medium): "Look, you’re almost 60 days overdue. We can’t keep waiting. If you don't pay the..." (similarity: 0.61)</t>
         </is>
       </c>
     </row>
@@ -7573,27 +7573,27 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>70.00%</t>
+          <t>72.00%</t>
         </is>
       </c>
       <c r="D179" t="inlineStr">
         <is>
-          <t>70.00%</t>
+          <t>75.00%</t>
         </is>
       </c>
       <c r="E179" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R003, R004, R005</t>
         </is>
       </c>
       <c r="F179" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>medium</t>
         </is>
       </c>
       <c r="G179" t="n">
@@ -7601,7 +7601,7 @@
       </c>
       <c r="H179" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R003 (high): "That's unfortunate, but you really should have thought about that before skippin..." (similarity: 0.61); R004 (medium): "That's unfortunate, but you really should have thought about that before skippin..." (similarity: 0.66); R005 (high): "Honestly, you're looking at serious consequences if this isn't taken care of soo..." (similarity: 0.72)</t>
         </is>
       </c>
     </row>
@@ -8053,27 +8053,27 @@
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>74.00%</t>
+          <t>66.00%</t>
         </is>
       </c>
       <c r="D191" t="inlineStr">
         <is>
-          <t>70.00%</t>
+          <t>75.00%</t>
         </is>
       </c>
       <c r="E191" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R001, R004</t>
         </is>
       </c>
       <c r="F191" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>medium</t>
         </is>
       </c>
       <c r="G191" t="n">
@@ -8081,7 +8081,7 @@
       </c>
       <c r="H191" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R001 (critical): "Well, that's not really our concern. You’re required to pay. If you don’t, we’ll..." (similarity: 0.63); R004 (medium): "Time is up, and we can't wait. You need to make a full payment now or face legal..." (similarity: 0.66)</t>
         </is>
       </c>
     </row>
@@ -8133,27 +8133,27 @@
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>74.00%</t>
+          <t>63.00%</t>
         </is>
       </c>
       <c r="D193" t="inlineStr">
         <is>
-          <t>70.00%</t>
+          <t>85.00%</t>
         </is>
       </c>
       <c r="E193" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R001</t>
         </is>
       </c>
       <c r="F193" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>critical</t>
         </is>
       </c>
       <c r="G193" t="n">
@@ -8161,7 +8161,7 @@
       </c>
       <c r="H193" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R001 (critical): "Look, I get it, but you signed the contract. If you don’t pay, we could just rep..." (similarity: 0.63)</t>
         </is>
       </c>
     </row>
@@ -8183,17 +8183,17 @@
       </c>
       <c r="D194" t="inlineStr">
         <is>
-          <t>85.00%</t>
+          <t>75.00%</t>
         </is>
       </c>
       <c r="E194" t="inlineStr">
         <is>
-          <t>R001</t>
+          <t>R001, R004</t>
         </is>
       </c>
       <c r="F194" t="inlineStr">
         <is>
-          <t>critical</t>
+          <t>medium</t>
         </is>
       </c>
       <c r="G194" t="n">
@@ -8201,7 +8201,7 @@
       </c>
       <c r="H194" t="inlineStr">
         <is>
-          <t>R001 (critical): "That’s unfortunate, but you still need to pay us. If you don’t pay by the end of..." (similarity: 0.66)</t>
+          <t>R001 (critical): "That’s unfortunate, but you still need to pay us. If you don’t pay by the end of..." (similarity: 0.66); R004 (medium): "That’s unfortunate, but you still need to pay us. If you don’t pay by the end of..." (similarity: 0.65)</t>
         </is>
       </c>
     </row>
@@ -8253,27 +8253,27 @@
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>72.00%</t>
+          <t>60.00%</t>
         </is>
       </c>
       <c r="D196" t="inlineStr">
         <is>
-          <t>70.00%</t>
+          <t>75.00%</t>
         </is>
       </c>
       <c r="E196" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R004</t>
         </is>
       </c>
       <c r="F196" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>medium</t>
         </is>
       </c>
       <c r="G196" t="n">
@@ -8281,7 +8281,7 @@
       </c>
       <c r="H196" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R004 (medium): "Look, if you don’t pay up immediately, your credit will tank and you’ll be facin..." (similarity: 0.60)</t>
         </is>
       </c>
     </row>
@@ -8293,27 +8293,27 @@
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="C197" t="inlineStr">
         <is>
-          <t>77.00%</t>
+          <t>60.00%</t>
         </is>
       </c>
       <c r="D197" t="inlineStr">
         <is>
-          <t>70.00%</t>
+          <t>75.00%</t>
         </is>
       </c>
       <c r="E197" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R004</t>
         </is>
       </c>
       <c r="F197" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>medium</t>
         </is>
       </c>
       <c r="G197" t="n">
@@ -8321,7 +8321,7 @@
       </c>
       <c r="H197" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R004 (medium): "I completely understand. We want to work with you during this time. Would you be..." (similarity: 0.60)</t>
         </is>
       </c>
     </row>
@@ -8333,27 +8333,27 @@
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>74.00%</t>
+          <t>67.00%</t>
         </is>
       </c>
       <c r="D198" t="inlineStr">
         <is>
-          <t>70.00%</t>
+          <t>75.00%</t>
         </is>
       </c>
       <c r="E198" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R004</t>
         </is>
       </c>
       <c r="F198" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>medium</t>
         </is>
       </c>
       <c r="G198" t="n">
@@ -8361,7 +8361,7 @@
       </c>
       <c r="H198" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R004 (medium): "I understand, but you really need to pay up immediately. If not, we’ll have to e..." (similarity: 0.67)</t>
         </is>
       </c>
     </row>
@@ -8373,27 +8373,27 @@
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>71.00%</t>
+          <t>64.00%</t>
         </is>
       </c>
       <c r="D199" t="inlineStr">
         <is>
-          <t>70.00%</t>
+          <t>75.00%</t>
         </is>
       </c>
       <c r="E199" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R002, R004</t>
         </is>
       </c>
       <c r="F199" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>medium</t>
         </is>
       </c>
       <c r="G199" t="n">
@@ -8401,7 +8401,7 @@
       </c>
       <c r="H199" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R002 (critical): "Time's not on your side. You need to commit to paying this debt now, or face the..." (similarity: 0.64); R004 (medium): "Well, you need to pay this off, or we'll have to take serious action. You can't ..." (similarity: 0.64)</t>
         </is>
       </c>
     </row>
@@ -8413,27 +8413,27 @@
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>73.00%</t>
+          <t>64.00%</t>
         </is>
       </c>
       <c r="D200" t="inlineStr">
         <is>
-          <t>70.00%</t>
+          <t>75.00%</t>
         </is>
       </c>
       <c r="E200" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R004</t>
         </is>
       </c>
       <c r="F200" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>medium</t>
         </is>
       </c>
       <c r="G200" t="n">
@@ -8441,7 +8441,7 @@
       </c>
       <c r="H200" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R004 (medium): "Well, you could have avoided this situation by paying on time. We are just follo..." (similarity: 0.64)</t>
         </is>
       </c>
     </row>
@@ -8468,7 +8468,7 @@
       </c>
       <c r="E201" t="inlineStr">
         <is>
-          <t>R004</t>
+          <t>R003, R004</t>
         </is>
       </c>
       <c r="F201" t="inlineStr">
@@ -8481,7 +8481,7 @@
       </c>
       <c r="H201" t="inlineStr">
         <is>
-          <t>R004 (medium): "I can't help you with that. If you don't pay immediately, we're going to report ..." (similarity: 0.72)</t>
+          <t>R003 (high): "I can't help you with that. If you don't pay immediately, we're going to report ..." (similarity: 0.61); R004 (medium): "I can't help you with that. If you don't pay immediately, we're going to report ..." (similarity: 0.72)</t>
         </is>
       </c>
     </row>

</xml_diff>